<commit_message>
Finish vt_lookup, add streamlit module to main
</commit_message>
<xml_diff>
--- a/output/threat_report.xlsx
+++ b/output/threat_report.xlsx
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -508,13 +508,13 @@
         <v>52</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="n">
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>